<commit_message>
Improvements to the balance of classification weight and additional sections to the report
</commit_message>
<xml_diff>
--- a/documentation/non-functional_requirements.xlsx
+++ b/documentation/non-functional_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ThomasFranklin/Tweet-Classification/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2C1542-2444-A642-A2B0-CCDE96FE2456}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B71FC4B-CC1E-9842-93F5-50B18B146AE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14960" xr2:uid="{56A7DCBB-48D4-8C4C-8F17-FD744938F507}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t xml:space="preserve">Relative Weights: </t>
   </si>
@@ -87,9 +87,6 @@
     <t>NF.04</t>
   </si>
   <si>
-    <t>System shall be accessible from a browser</t>
-  </si>
-  <si>
     <t>NF.05</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
   </si>
   <si>
     <t>System shall give user a response within 5 seconds of navigating to a page</t>
-  </si>
-  <si>
-    <t>NF.10</t>
   </si>
   <si>
     <t>System shall be developed using best practices</t>
@@ -522,18 +516,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A28E84-601A-4F42-BC57-826D827B8885}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="O22:Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="6"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="9.5" customWidth="1"/>
+    <col min="16" max="16" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="34" x14ac:dyDescent="0.2">
@@ -611,26 +605,26 @@
         <v>27</v>
       </c>
       <c r="F3" s="2">
-        <f>ROUND(E3/E$13,2)</f>
-        <v>0.11</v>
+        <f>ROUND(E3/E$12,2)</f>
+        <v>0.12</v>
       </c>
       <c r="G3" s="2">
         <v>3</v>
       </c>
       <c r="H3" s="2">
-        <f>ROUND(G3/G$13,2)</f>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(G3/G$12,2)</f>
+        <v>0.08</v>
       </c>
       <c r="I3" s="2">
         <v>4</v>
       </c>
       <c r="J3" s="2">
-        <f>ROUND(I3/I$13,2)</f>
-        <v>0.08</v>
+        <f>ROUND(I3/I$12,2)</f>
+        <v>0.09</v>
       </c>
       <c r="K3" s="2">
         <f>ROUND((F3)/(H3*0+J3*I$1),2)</f>
-        <v>0.69</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="153" x14ac:dyDescent="0.2">
@@ -651,34 +645,34 @@
         <v>27</v>
       </c>
       <c r="F4" s="2">
-        <f>ROUND(E4/E$13,2)</f>
-        <v>0.11</v>
+        <f>ROUND(E4/E$12,2)</f>
+        <v>0.12</v>
       </c>
       <c r="G4" s="2">
         <v>9</v>
       </c>
       <c r="H4" s="2">
-        <f>ROUND(G4/G$13,2)</f>
-        <v>0.21</v>
+        <f>ROUND(G4/G$12,2)</f>
+        <v>0.23</v>
       </c>
       <c r="I4" s="2">
         <v>5</v>
       </c>
       <c r="J4" s="2">
-        <f>ROUND(I4/I$13,2)</f>
-        <v>0.1</v>
+        <f>ROUND(I4/I$12,2)</f>
+        <v>0.11</v>
       </c>
       <c r="K4" s="2">
         <f>ROUND((F4)/(H4*0+J4*I$1),2)</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>9</v>
@@ -691,26 +685,26 @@
         <v>27</v>
       </c>
       <c r="F5" s="2">
-        <f>ROUND(E5/E$13,2)</f>
-        <v>0.11</v>
+        <f>ROUND(E5/E$12,2)</f>
+        <v>0.12</v>
       </c>
       <c r="G5" s="2">
         <v>3</v>
       </c>
       <c r="H5" s="2">
-        <f>ROUND(G5/G$13,2)</f>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(G5/G$12,2)</f>
+        <v>0.08</v>
       </c>
       <c r="I5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" s="2">
-        <f>ROUND(I5/I$13,2)</f>
-        <v>0.06</v>
+        <f>ROUND(I5/I$12,2)</f>
+        <v>0.09</v>
       </c>
       <c r="K5" s="2">
         <f>ROUND((F5)/(H5*0+J5*I$1),2)</f>
-        <v>0.92</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="102" x14ac:dyDescent="0.2">
@@ -718,47 +712,47 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <v>9</v>
       </c>
       <c r="D6" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2">
         <f>(C6*C$1)+D6*D$1</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2">
-        <f>ROUND(E6/E$13,2)</f>
-        <v>0.11</v>
+        <f>ROUND(E6/E$12,2)</f>
+        <v>0.1</v>
       </c>
       <c r="G6" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H6" s="2">
-        <f>ROUND(G6/G$13,2)</f>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(G6/G$12,2)</f>
+        <v>0.23</v>
       </c>
       <c r="I6" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J6" s="2">
-        <f>ROUND(I6/I$13,2)</f>
-        <v>0.08</v>
+        <f>ROUND(I6/I$12,2)</f>
+        <v>0.16</v>
       </c>
       <c r="K6" s="2">
         <f>ROUND((F6)/(H6*0+J6*I$1),2)</f>
-        <v>0.69</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2">
         <v>9</v>
@@ -771,151 +765,151 @@
         <v>22</v>
       </c>
       <c r="F7" s="2">
-        <f>ROUND(E7/E$13,2)</f>
-        <v>0.09</v>
+        <f>ROUND(E7/E$12,2)</f>
+        <v>0.1</v>
       </c>
       <c r="G7" s="2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2">
-        <f>ROUND(G7/G$13,2)</f>
-        <v>0.21</v>
+        <f>ROUND(G7/G$12,2)</f>
+        <v>0.08</v>
       </c>
       <c r="I7" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J7" s="2">
-        <f>ROUND(I7/I$13,2)</f>
-        <v>0.15</v>
+        <f>ROUND(I7/I$12,2)</f>
+        <v>0.11</v>
       </c>
       <c r="K7" s="2">
         <f>ROUND((F7)/(H7*0+J7*I$1),2)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2">
         <v>9</v>
       </c>
       <c r="D8" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8" s="2">
         <f>(C8*C$1)+D8*D$1</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2">
-        <f>ROUND(E8/E$13,2)</f>
-        <v>0.09</v>
+        <f>ROUND(E8/E$12,2)</f>
+        <v>0.11</v>
       </c>
       <c r="G8" s="2">
         <v>3</v>
       </c>
       <c r="H8" s="2">
-        <f>ROUND(G8/G$13,2)</f>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(G8/G$12,2)</f>
+        <v>0.08</v>
       </c>
       <c r="I8" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J8" s="2">
-        <f>ROUND(I8/I$13,2)</f>
-        <v>0.1</v>
+        <f>ROUND(I8/I$12,2)</f>
+        <v>0.09</v>
       </c>
       <c r="K8" s="2">
         <f>ROUND((F8)/(H8*0+J8*I$1),2)</f>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2">
         <v>6</v>
       </c>
       <c r="E9" s="2">
         <f>(C9*C$1)+D9*D$1</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2">
-        <f>ROUND(E9/E$13,2)</f>
-        <v>0.1</v>
+        <f>ROUND(E9/E$12,2)</f>
+        <v>0.08</v>
       </c>
       <c r="G9" s="2">
         <v>3</v>
       </c>
       <c r="H9" s="2">
-        <f>ROUND(G9/G$13,2)</f>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(G9/G$12,2)</f>
+        <v>0.08</v>
       </c>
       <c r="I9" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J9" s="2">
-        <f>ROUND(I9/I$13,2)</f>
-        <v>0.08</v>
+        <f>ROUND(I9/I$12,2)</f>
+        <v>0.16</v>
       </c>
       <c r="K9" s="2">
         <f>ROUND((F9)/(H9*0+J9*I$1),2)</f>
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
         <f>(C10*C$1)+D10*D$1</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2">
-        <f>ROUND(E10/E$13,2)</f>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(E10/E$12,2)</f>
+        <v>0.11</v>
       </c>
       <c r="G10" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" s="2">
-        <f>ROUND(G10/G$13,2)</f>
-        <v>7.0000000000000007E-2</v>
+        <f>ROUND(G10/G$12,2)</f>
+        <v>0.1</v>
       </c>
       <c r="I10" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J10" s="2">
-        <f>ROUND(I10/I$13,2)</f>
-        <v>0.15</v>
+        <f>ROUND(I10/I$12,2)</f>
+        <v>0.11</v>
       </c>
       <c r="K10" s="2">
         <f>ROUND((F10)/(H10*0+J10*I$1),2)</f>
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="136" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>30</v>
@@ -924,109 +918,74 @@
         <v>9</v>
       </c>
       <c r="D11" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
         <f>(C11*C$1)+D11*D$1</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2">
-        <f>ROUND(E11/E$13,2)</f>
-        <v>0.1</v>
+        <f>ROUND(E11/E$12,2)</f>
+        <v>0.12</v>
       </c>
       <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <f>ROUND(G11/G$12,2)</f>
+        <v>0.05</v>
+      </c>
+      <c r="I11" s="2">
         <v>4</v>
       </c>
-      <c r="H11" s="2">
-        <f>ROUND(G11/G$13,2)</f>
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="2">
-        <v>5</v>
-      </c>
       <c r="J11" s="2">
-        <f>ROUND(I11/I$13,2)</f>
-        <v>0.1</v>
+        <f>ROUND(I11/I$12,2)</f>
+        <v>0.09</v>
       </c>
       <c r="K11" s="2">
         <f>ROUND((F11)/(H11*0+J11*I$1),2)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="23" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
+        <f>SUM(C3:C3)</f>
         <v>9</v>
       </c>
       <c r="D12" s="2">
+        <f>SUM(D3:D3)</f>
         <v>9</v>
       </c>
       <c r="E12" s="2">
-        <f>(C12*C$1)+D12*D$1</f>
-        <v>27</v>
+        <f>SUM(E3:E11)</f>
+        <v>219</v>
       </c>
       <c r="F12" s="2">
-        <f>ROUND(E12/E$13,2)</f>
-        <v>0.11</v>
+        <v>100</v>
       </c>
       <c r="G12" s="2">
-        <v>2</v>
+        <f>SUM(G3:G11)</f>
+        <v>39</v>
       </c>
       <c r="H12" s="2">
-        <f>ROUND(G12/G$13,2)</f>
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="I12" s="2">
-        <v>4</v>
+        <f>SUM(I3:I11)</f>
+        <v>45</v>
       </c>
       <c r="J12" s="2">
-        <f>ROUND(I12/I$13,2)</f>
-        <v>0.08</v>
-      </c>
-      <c r="K12" s="2">
-        <f>ROUND((F12)/(H12*0+J12*I$1),2)</f>
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="23" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2">
-        <f>SUM(C3:C3)</f>
-        <v>9</v>
-      </c>
-      <c r="D13" s="2">
-        <f>SUM(D3:D3)</f>
-        <v>9</v>
-      </c>
-      <c r="E13" s="2">
-        <f>SUM(E3:E12)</f>
-        <v>246</v>
-      </c>
-      <c r="F13" s="2">
         <v>100</v>
       </c>
-      <c r="G13" s="2">
-        <f>SUM(G3:G12)</f>
-        <v>42</v>
-      </c>
-      <c r="H13" s="2">
-        <v>100</v>
-      </c>
-      <c r="I13" s="2">
-        <f>SUM(I3:I12)</f>
-        <v>48</v>
-      </c>
-      <c r="J13" s="2">
-        <v>100</v>
-      </c>
-      <c r="K13" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="O13" s="6"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
@@ -1072,19 +1031,108 @@
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="15:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="O22" s="6"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="2"/>
+      <c r="O22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="23" spans="15:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="O23" s="6"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="2"/>
+      <c r="O23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
     <row r="24" spans="15:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="O24" s="6"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="2"/>
+      <c r="O24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="25" spans="15:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="O25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="26" spans="15:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="O26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="27" spans="15:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="O27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="28" spans="15:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="O28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="15:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="O29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="15:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="O30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="31" spans="15:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="O31" s="6"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>